<commit_message>
Including SvyID in the input table
</commit_message>
<xml_diff>
--- a/RTM_pipeline_input.xlsx
+++ b/RTM_pipeline_input.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="25601"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26130"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://wfp.sharepoint.com/sites/RBC-Nearreal-timemonitoringsystem/Shared Documents/mVAM regular activities/Regional/RTM modified standard pipeline/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="2" documentId="13_ncr:1_{A0F397BA-F704-4431-AE13-DA07760DCFC8}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{02BCCEC4-447A-424F-9F76-54E7BE46C64A}"/>
+  <xr:revisionPtr revIDLastSave="11" documentId="13_ncr:1_{A0F397BA-F704-4431-AE13-DA07760DCFC8}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{4F506A77-F5F4-4918-A259-550A51766D9A}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="25820" windowHeight="14020" xr2:uid="{D20F4FC1-04AB-4C77-B328-DEC9A7A24BBA}"/>
   </bookViews>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="14" uniqueCount="10">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="15" uniqueCount="11">
   <si>
     <t>CountryCode</t>
   </si>
@@ -66,6 +66,9 @@
   </si>
   <si>
     <t>Yemen1</t>
+  </si>
+  <si>
+    <t xml:space="preserve">SvyID </t>
   </si>
 </sst>
 </file>
@@ -418,10 +421,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C57113FC-800F-4C38-A619-9E09C8B14E96}">
-  <dimension ref="A1:E4"/>
+  <dimension ref="A1:F4"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F8" sqref="F8"/>
+      <selection activeCell="L12" sqref="L12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -431,7 +434,7 @@
     <col min="4" max="5" width="10.453125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A1" t="s">
         <v>3</v>
       </c>
@@ -447,8 +450,11 @@
       <c r="E1" t="s">
         <v>2</v>
       </c>
+      <c r="F1" t="s">
+        <v>10</v>
+      </c>
     </row>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A2" t="s">
         <v>5</v>
       </c>
@@ -462,10 +468,13 @@
         <v>45078</v>
       </c>
       <c r="E2" s="1">
-        <v>45092</v>
+        <v>45103</v>
+      </c>
+      <c r="F2">
+        <v>333</v>
       </c>
     </row>
-    <row r="3" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A3" t="s">
         <v>5</v>
       </c>
@@ -479,10 +488,13 @@
         <v>45078</v>
       </c>
       <c r="E3" s="1">
-        <v>45095</v>
+        <v>45103</v>
+      </c>
+      <c r="F3">
+        <v>10044</v>
       </c>
     </row>
-    <row r="4" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A4" t="s">
         <v>5</v>
       </c>
@@ -496,7 +508,10 @@
         <v>45078</v>
       </c>
       <c r="E4" s="1">
-        <v>45095</v>
+        <v>45131</v>
+      </c>
+      <c r="F4">
+        <v>109</v>
       </c>
     </row>
   </sheetData>
@@ -515,17 +530,8 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
-</file>
-
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
-<ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Document" ma:contentTypeID="0x010100078FB844456CC1439CE7A159479264B8" ma:contentTypeVersion="4" ma:contentTypeDescription="Create a new document." ma:contentTypeScope="" ma:versionID="12760576e647fd099db26633cd98c847">
-  <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns2="df49477f-2fdb-440d-ba1e-675744a510a7" xmlns:ns3="272bea84-3b1f-4555-a3af-524feb91c688" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="4d9fb2268678995e8d267809d44d0327" ns2:_="" ns3:_="">
+<ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Document" ma:contentTypeID="0x010100078FB844456CC1439CE7A159479264B8" ma:contentTypeVersion="5" ma:contentTypeDescription="Create a new document." ma:contentTypeScope="" ma:versionID="996a4699cbb302f4d95a15d67d32f7e1">
+  <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns2="df49477f-2fdb-440d-ba1e-675744a510a7" xmlns:ns3="272bea84-3b1f-4555-a3af-524feb91c688" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="ebe6ffb6dba8b9d24d4c1cd32a9bdc8d" ns2:_="" ns3:_="">
     <xsd:import namespace="df49477f-2fdb-440d-ba1e-675744a510a7"/>
     <xsd:import namespace="272bea84-3b1f-4555-a3af-524feb91c688"/>
     <xsd:element name="properties">
@@ -538,6 +544,7 @@
                 <xsd:element ref="ns2:MediaServiceFastMetadata" minOccurs="0"/>
                 <xsd:element ref="ns3:SharedWithUsers" minOccurs="0"/>
                 <xsd:element ref="ns3:SharedWithDetails" minOccurs="0"/>
+                <xsd:element ref="ns2:MediaServiceObjectDetectorVersions" minOccurs="0"/>
               </xsd:all>
             </xsd:complexType>
           </xsd:element>
@@ -556,6 +563,11 @@
     <xsd:element name="MediaServiceFastMetadata" ma:index="9" nillable="true" ma:displayName="MediaServiceFastMetadata" ma:hidden="true" ma:internalName="MediaServiceFastMetadata" ma:readOnly="true">
       <xsd:simpleType>
         <xsd:restriction base="dms:Note"/>
+      </xsd:simpleType>
+    </xsd:element>
+    <xsd:element name="MediaServiceObjectDetectorVersions" ma:index="12" nillable="true" ma:displayName="MediaServiceObjectDetectorVersions" ma:hidden="true" ma:indexed="true" ma:internalName="MediaServiceObjectDetectorVersions" ma:readOnly="true">
+      <xsd:simpleType>
+        <xsd:restriction base="dms:Text"/>
       </xsd:simpleType>
     </xsd:element>
   </xsd:schema>
@@ -688,16 +700,23 @@
 </ct:contentTypeSchema>
 </file>
 
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement/>
+</p:properties>
+</file>
+
+<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
+</file>
+
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{C4C492B7-1129-41A1-824F-AF2B4F0C3BD3}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{E8A42D6A-F70E-41C6-9574-33CBEBAFA01C}">
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{40D87B69-39D5-493B-A16C-F1F1A2E9E303}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes"/>
@@ -713,4 +732,21 @@
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/internal/obd"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
+</file>
+
+<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{BF3E4F3B-1E48-447B-9CCB-C7ABB5D25424}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
+</file>
+
+<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{C4C492B7-1129-41A1-824F-AF2B4F0C3BD3}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
</xml_diff>

<commit_message>
variables names mapping automation
</commit_message>
<xml_diff>
--- a/RTM_pipeline_input.xlsx
+++ b/RTM_pipeline_input.xlsx
@@ -8,12 +8,13 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://wfp.sharepoint.com/sites/RBC-Nearreal-timemonitoringsystem/Shared Documents/mVAM regular activities/Regional/RTM modified standard pipeline/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="11" documentId="13_ncr:1_{A0F397BA-F704-4431-AE13-DA07760DCFC8}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{4F506A77-F5F4-4918-A259-550A51766D9A}"/>
+  <xr:revisionPtr revIDLastSave="154" documentId="13_ncr:1_{A0F397BA-F704-4431-AE13-DA07760DCFC8}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{7403BA93-D72A-4B7C-8CA0-62E10183472F}"/>
   <bookViews>
-    <workbookView xWindow="-110" yWindow="-110" windowWidth="25820" windowHeight="14020" xr2:uid="{D20F4FC1-04AB-4C77-B328-DEC9A7A24BBA}"/>
+    <workbookView xWindow="-96" yWindow="-96" windowWidth="23232" windowHeight="12552" activeTab="1" xr2:uid="{D20F4FC1-04AB-4C77-B328-DEC9A7A24BBA}"/>
   </bookViews>
   <sheets>
-    <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
+    <sheet name="main_parameters" sheetId="1" r:id="rId1"/>
+    <sheet name="standard_names_mapping" sheetId="2" r:id="rId2"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -36,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="15" uniqueCount="11">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="330" uniqueCount="123">
   <si>
     <t>CountryCode</t>
   </si>
@@ -69,19 +70,366 @@
   </si>
   <si>
     <t xml:space="preserve">SvyID </t>
+  </si>
+  <si>
+    <t>Others</t>
+  </si>
+  <si>
+    <t>Libya</t>
+  </si>
+  <si>
+    <t>Orignial</t>
+  </si>
+  <si>
+    <t>Standard</t>
+  </si>
+  <si>
+    <t>Country</t>
+  </si>
+  <si>
+    <t>City</t>
+  </si>
+  <si>
+    <t>Area</t>
+  </si>
+  <si>
+    <t>LogDate1</t>
+  </si>
+  <si>
+    <t>Agent</t>
+  </si>
+  <si>
+    <t>HouseType</t>
+  </si>
+  <si>
+    <t>ADMIN0Name</t>
+  </si>
+  <si>
+    <t>ADMIN1Name</t>
+  </si>
+  <si>
+    <t>ADMIN2Name</t>
+  </si>
+  <si>
+    <t>ObsDate</t>
+  </si>
+  <si>
+    <t>EnuName</t>
+  </si>
+  <si>
+    <t>HDwellType</t>
+  </si>
+  <si>
+    <t>Yemen</t>
+  </si>
+  <si>
+    <t>HoHSex</t>
+  </si>
+  <si>
+    <t>HHHSex</t>
+  </si>
+  <si>
+    <t>HHSize_90days</t>
+  </si>
+  <si>
+    <t>HHSize</t>
+  </si>
+  <si>
+    <t>HHDispl</t>
+  </si>
+  <si>
+    <t>BirthYear</t>
+  </si>
+  <si>
+    <t>RESPAge</t>
+  </si>
+  <si>
+    <t>HH65_Disease</t>
+  </si>
+  <si>
+    <t>HHChronIllNb</t>
+  </si>
+  <si>
+    <t>Staples</t>
+  </si>
+  <si>
+    <t>FCSStap</t>
+  </si>
+  <si>
+    <t>Pulses</t>
+  </si>
+  <si>
+    <t>FCSPulse</t>
+  </si>
+  <si>
+    <t>Veg</t>
+  </si>
+  <si>
+    <t>FCSVeg</t>
+  </si>
+  <si>
+    <t>Fruits</t>
+  </si>
+  <si>
+    <t>FCSFruit</t>
+  </si>
+  <si>
+    <t>Proteins</t>
+  </si>
+  <si>
+    <t>FCSPr</t>
+  </si>
+  <si>
+    <t>Dairy</t>
+  </si>
+  <si>
+    <t>FCSDairy</t>
+  </si>
+  <si>
+    <t>Fats</t>
+  </si>
+  <si>
+    <t>FCSFat</t>
+  </si>
+  <si>
+    <t>Sugars</t>
+  </si>
+  <si>
+    <t>FCSSugar</t>
+  </si>
+  <si>
+    <t>FoodSrc1</t>
+  </si>
+  <si>
+    <t>FCS_SRf</t>
+  </si>
+  <si>
+    <t>LessExpensiveFood</t>
+  </si>
+  <si>
+    <t>rCSILessQlty</t>
+  </si>
+  <si>
+    <t>BorrowOrHelp</t>
+  </si>
+  <si>
+    <t>rCSIBorrow</t>
+  </si>
+  <si>
+    <t>ReduceNumMeals</t>
+  </si>
+  <si>
+    <t>rCSIMealNb</t>
+  </si>
+  <si>
+    <t>LimitPortionSize</t>
+  </si>
+  <si>
+    <t>rCSIMealSize</t>
+  </si>
+  <si>
+    <t>RestrictConsumption</t>
+  </si>
+  <si>
+    <t>rCSIMealAdult</t>
+  </si>
+  <si>
+    <t>Income_MainSrc</t>
+  </si>
+  <si>
+    <t>HHIncFirst_SRi</t>
+  </si>
+  <si>
+    <t>Income_Change</t>
+  </si>
+  <si>
+    <t>HHIncChg_1M</t>
+  </si>
+  <si>
+    <t>LC_2_SoldAsset</t>
+  </si>
+  <si>
+    <t>LcsEN_stress_DomAsset</t>
+  </si>
+  <si>
+    <t>LC_3_CreditFood</t>
+  </si>
+  <si>
+    <t>LcsEN_stress_CrdtFood</t>
+  </si>
+  <si>
+    <t>LC_4_SpentSaving</t>
+  </si>
+  <si>
+    <t>LcsEN_stress_Saving</t>
+  </si>
+  <si>
+    <t>LC_5_BorrowMoney</t>
+  </si>
+  <si>
+    <t>LcsEN_stress_BorrowCash</t>
+  </si>
+  <si>
+    <t>LC_6_SoldProduction</t>
+  </si>
+  <si>
+    <t>LcsEN_crisis_ProdAssets</t>
+  </si>
+  <si>
+    <t>LC_7_ReduceHealth</t>
+  </si>
+  <si>
+    <t>LcsEN_crisis_Health</t>
+  </si>
+  <si>
+    <t>LC_8_WithdrawSchool</t>
+  </si>
+  <si>
+    <t>LcsEN_crisis_OutSchool</t>
+  </si>
+  <si>
+    <t>LC_9_SoldHome</t>
+  </si>
+  <si>
+    <t>LcsEN_em_ResAsset</t>
+  </si>
+  <si>
+    <t>LC_10_Begged</t>
+  </si>
+  <si>
+    <t>LcsEN_em_Begged</t>
+  </si>
+  <si>
+    <t>LhCSIEnAccess</t>
+  </si>
+  <si>
+    <t>LC_11_LastAnimal</t>
+  </si>
+  <si>
+    <t>LcsEN_em_LastAnimal</t>
+  </si>
+  <si>
+    <t>RespNationality</t>
+  </si>
+  <si>
+    <t>DispStat_Nationality</t>
+  </si>
+  <si>
+    <t>HoHH_Sex</t>
+  </si>
+  <si>
+    <t>HWaterSRC</t>
+  </si>
+  <si>
+    <t>HHdrinkingwater</t>
+  </si>
+  <si>
+    <t>HToiletType</t>
+  </si>
+  <si>
+    <t>HHtoiletfacility</t>
+  </si>
+  <si>
+    <t>HElectricitySRC</t>
+  </si>
+  <si>
+    <t>MainSourcesElectricity</t>
+  </si>
+  <si>
+    <t>HHHousingCurrent</t>
+  </si>
+  <si>
+    <t>HHFoodSource</t>
+  </si>
+  <si>
+    <t>Lcs_stress_DomAsset</t>
+  </si>
+  <si>
+    <t>LhCSIDomAsset</t>
+  </si>
+  <si>
+    <t>Lcs_stress_CrdtFood</t>
+  </si>
+  <si>
+    <t>LhCSICrdtFood</t>
+  </si>
+  <si>
+    <t>Lcs_crisis_ProdAssets</t>
+  </si>
+  <si>
+    <t>LhCSIProdAsset</t>
+  </si>
+  <si>
+    <t>LhCSIsoldhouse</t>
+  </si>
+  <si>
+    <t>Lcs_em_ResAsset</t>
+  </si>
+  <si>
+    <t>Lcs_stress_BorrowCash</t>
+  </si>
+  <si>
+    <t>LhCSIBorrowCash</t>
+  </si>
+  <si>
+    <t>Lcs_stress_LessSchool</t>
+  </si>
+  <si>
+    <t>LhCSIchangedschool</t>
+  </si>
+  <si>
+    <t>LhCSIOutSchool</t>
+  </si>
+  <si>
+    <t>Lcs_crisis_OutSchool</t>
+  </si>
+  <si>
+    <t>Lcs_crisis_Health</t>
+  </si>
+  <si>
+    <t>LhCSIHealth</t>
+  </si>
+  <si>
+    <t>Lcs_em_Begged</t>
+  </si>
+  <si>
+    <t>LhCSIBegged</t>
+  </si>
+  <si>
+    <t>Included</t>
+  </si>
+  <si>
+    <t>Y</t>
+  </si>
+  <si>
+    <t>IDP_YN</t>
+  </si>
+  <si>
+    <t>LC_MainReason</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="1" x14ac:knownFonts="1">
+  <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF000000"/>
+      <name val="Calibri"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF000000"/>
+      <name val="Calibri"/>
+      <family val="2"/>
     </font>
   </fonts>
   <fills count="2">
@@ -92,7 +440,7 @@
       <patternFill patternType="gray125"/>
     </fill>
   </fills>
-  <borders count="1">
+  <borders count="3">
     <border>
       <left/>
       <right/>
@@ -100,18 +448,97 @@
       <bottom/>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color rgb="FF000000"/>
+      </left>
+      <right style="thin">
+        <color rgb="FF000000"/>
+      </right>
+      <top style="thin">
+        <color rgb="FF000000"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="FF000000"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="FF000000"/>
+      </left>
+      <right style="thin">
+        <color rgb="FF000000"/>
+      </right>
+      <top style="thin">
+        <color rgb="FF000000"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="8">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="0"/>
+  <dxfs count="1">
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="11"/>
+        <color rgb="FF000000"/>
+        <name val="Calibri"/>
+        <scheme val="none"/>
+      </font>
+      <alignment horizontal="left" vertical="top" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <border diagonalUp="0" diagonalDown="0">
+        <left style="thin">
+          <color rgb="FF000000"/>
+        </left>
+        <right style="thin">
+          <color rgb="FF000000"/>
+        </right>
+        <top style="thin">
+          <color rgb="FF000000"/>
+        </top>
+        <bottom style="thin">
+          <color rgb="FF000000"/>
+        </bottom>
+        <vertical/>
+        <horizontal/>
+      </border>
+    </dxf>
+  </dxfs>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
@@ -122,6 +549,19 @@
     </ext>
   </extLst>
 </styleSheet>
+</file>
+
+<file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{D6F7B24D-0E6C-46A3-95CE-35EB22D1B624}" name="Table1" displayName="Table1" ref="A1:D78" totalsRowShown="0">
+  <autoFilter ref="A1:D78" xr:uid="{D6F7B24D-0E6C-46A3-95CE-35EB22D1B624}"/>
+  <tableColumns count="4">
+    <tableColumn id="1" xr3:uid="{76AE06AD-D71E-438E-BE0C-351F7C48C07B}" name="Country"/>
+    <tableColumn id="2" xr3:uid="{99EC5D9B-2587-4003-B89C-7482B8D22BAF}" name="Orignial"/>
+    <tableColumn id="3" xr3:uid="{AF765A21-27F3-4AC3-935C-1A26890B6581}" name="Standard" dataDxfId="0"/>
+    <tableColumn id="4" xr3:uid="{76AC2109-0758-47C8-8124-CE277C3DDAC6}" name="Included"/>
+  </tableColumns>
+  <tableStyleInfo name="TableStyleLight8" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
+</table>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -421,20 +861,20 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C57113FC-800F-4C38-A619-9E09C8B14E96}">
-  <dimension ref="A1:F4"/>
+  <dimension ref="A1:F5"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="L12" sqref="L12"/>
+    <sheetView zoomScale="140" zoomScaleNormal="140" workbookViewId="0">
+      <selection activeCell="D9" sqref="D9"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.55000000000000004"/>
   <cols>
-    <col min="2" max="2" width="10.36328125" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="11.7265625" bestFit="1" customWidth="1"/>
-    <col min="4" max="5" width="10.453125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="10.3671875" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="11.734375" bestFit="1" customWidth="1"/>
+    <col min="4" max="5" width="10.47265625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:6" x14ac:dyDescent="0.55000000000000004">
       <c r="A1" t="s">
         <v>3</v>
       </c>
@@ -454,7 +894,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="2" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:6" x14ac:dyDescent="0.55000000000000004">
       <c r="A2" t="s">
         <v>5</v>
       </c>
@@ -465,16 +905,16 @@
         <v>7</v>
       </c>
       <c r="D2" s="1">
-        <v>45078</v>
+        <v>45108</v>
       </c>
       <c r="E2" s="1">
-        <v>45103</v>
+        <v>45138</v>
       </c>
       <c r="F2">
         <v>333</v>
       </c>
     </row>
-    <row r="3" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:6" x14ac:dyDescent="0.55000000000000004">
       <c r="A3" t="s">
         <v>5</v>
       </c>
@@ -485,16 +925,16 @@
         <v>9</v>
       </c>
       <c r="D3" s="1">
-        <v>45078</v>
+        <v>45108</v>
       </c>
       <c r="E3" s="1">
-        <v>45103</v>
+        <v>45138</v>
       </c>
       <c r="F3">
         <v>10044</v>
       </c>
     </row>
-    <row r="4" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:6" x14ac:dyDescent="0.55000000000000004">
       <c r="A4" t="s">
         <v>5</v>
       </c>
@@ -512,6 +952,26 @@
       </c>
       <c r="F4">
         <v>109</v>
+      </c>
+    </row>
+    <row r="5" spans="1:6" x14ac:dyDescent="0.55000000000000004">
+      <c r="A5" t="s">
+        <v>5</v>
+      </c>
+      <c r="B5" t="s">
+        <v>11</v>
+      </c>
+      <c r="C5" t="s">
+        <v>12</v>
+      </c>
+      <c r="D5" s="1">
+        <v>45119</v>
+      </c>
+      <c r="E5" s="1">
+        <v>45133</v>
+      </c>
+      <c r="F5">
+        <v>1003</v>
       </c>
     </row>
   </sheetData>
@@ -529,9 +989,1134 @@
 </worksheet>
 </file>
 
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{1C3F78F6-9E57-4B5C-A811-BA52C216BE17}">
+  <dimension ref="A1:D78"/>
+  <sheetViews>
+    <sheetView tabSelected="1" topLeftCell="A29" workbookViewId="0">
+      <selection activeCell="B33" sqref="B33"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.55000000000000004"/>
+  <cols>
+    <col min="1" max="1" width="10.15625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="26.41796875" customWidth="1"/>
+    <col min="3" max="3" width="21.47265625" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:4" x14ac:dyDescent="0.55000000000000004">
+      <c r="A1" t="s">
+        <v>15</v>
+      </c>
+      <c r="B1" t="s">
+        <v>13</v>
+      </c>
+      <c r="C1" t="s">
+        <v>14</v>
+      </c>
+      <c r="D1" t="s">
+        <v>119</v>
+      </c>
+    </row>
+    <row r="2" spans="1:4" x14ac:dyDescent="0.55000000000000004">
+      <c r="A2" t="s">
+        <v>7</v>
+      </c>
+      <c r="B2" t="s">
+        <v>15</v>
+      </c>
+      <c r="C2" t="s">
+        <v>21</v>
+      </c>
+      <c r="D2" t="s">
+        <v>120</v>
+      </c>
+    </row>
+    <row r="3" spans="1:4" x14ac:dyDescent="0.55000000000000004">
+      <c r="A3" t="s">
+        <v>7</v>
+      </c>
+      <c r="B3" t="s">
+        <v>16</v>
+      </c>
+      <c r="C3" t="s">
+        <v>22</v>
+      </c>
+      <c r="D3" t="s">
+        <v>120</v>
+      </c>
+    </row>
+    <row r="4" spans="1:4" x14ac:dyDescent="0.55000000000000004">
+      <c r="A4" t="s">
+        <v>7</v>
+      </c>
+      <c r="B4" t="s">
+        <v>17</v>
+      </c>
+      <c r="C4" t="s">
+        <v>23</v>
+      </c>
+      <c r="D4" t="s">
+        <v>120</v>
+      </c>
+    </row>
+    <row r="5" spans="1:4" x14ac:dyDescent="0.55000000000000004">
+      <c r="A5" t="s">
+        <v>7</v>
+      </c>
+      <c r="B5" t="s">
+        <v>18</v>
+      </c>
+      <c r="C5" t="s">
+        <v>24</v>
+      </c>
+      <c r="D5" t="s">
+        <v>120</v>
+      </c>
+    </row>
+    <row r="6" spans="1:4" x14ac:dyDescent="0.55000000000000004">
+      <c r="A6" t="s">
+        <v>7</v>
+      </c>
+      <c r="B6" t="s">
+        <v>19</v>
+      </c>
+      <c r="C6" t="s">
+        <v>25</v>
+      </c>
+      <c r="D6" t="s">
+        <v>120</v>
+      </c>
+    </row>
+    <row r="7" spans="1:4" x14ac:dyDescent="0.55000000000000004">
+      <c r="A7" t="s">
+        <v>7</v>
+      </c>
+      <c r="B7" t="s">
+        <v>20</v>
+      </c>
+      <c r="C7" t="s">
+        <v>26</v>
+      </c>
+      <c r="D7" t="s">
+        <v>120</v>
+      </c>
+    </row>
+    <row r="8" spans="1:4" x14ac:dyDescent="0.55000000000000004">
+      <c r="A8" t="s">
+        <v>27</v>
+      </c>
+      <c r="B8" t="s">
+        <v>18</v>
+      </c>
+      <c r="C8" t="s">
+        <v>24</v>
+      </c>
+      <c r="D8" t="s">
+        <v>120</v>
+      </c>
+    </row>
+    <row r="9" spans="1:4" x14ac:dyDescent="0.55000000000000004">
+      <c r="A9" t="s">
+        <v>27</v>
+      </c>
+      <c r="B9" t="s">
+        <v>19</v>
+      </c>
+      <c r="C9" t="s">
+        <v>25</v>
+      </c>
+      <c r="D9" t="s">
+        <v>120</v>
+      </c>
+    </row>
+    <row r="10" spans="1:4" x14ac:dyDescent="0.55000000000000004">
+      <c r="A10" t="s">
+        <v>27</v>
+      </c>
+      <c r="B10" t="s">
+        <v>15</v>
+      </c>
+      <c r="C10" t="s">
+        <v>21</v>
+      </c>
+      <c r="D10" t="s">
+        <v>120</v>
+      </c>
+    </row>
+    <row r="11" spans="1:4" x14ac:dyDescent="0.55000000000000004">
+      <c r="A11" t="s">
+        <v>27</v>
+      </c>
+      <c r="B11" t="s">
+        <v>16</v>
+      </c>
+      <c r="C11" t="s">
+        <v>22</v>
+      </c>
+      <c r="D11" t="s">
+        <v>120</v>
+      </c>
+    </row>
+    <row r="12" spans="1:4" x14ac:dyDescent="0.55000000000000004">
+      <c r="A12" t="s">
+        <v>27</v>
+      </c>
+      <c r="B12" t="s">
+        <v>17</v>
+      </c>
+      <c r="C12" t="s">
+        <v>23</v>
+      </c>
+      <c r="D12" t="s">
+        <v>120</v>
+      </c>
+    </row>
+    <row r="13" spans="1:4" x14ac:dyDescent="0.55000000000000004">
+      <c r="A13" t="s">
+        <v>27</v>
+      </c>
+      <c r="B13" t="s">
+        <v>28</v>
+      </c>
+      <c r="C13" s="2" t="s">
+        <v>29</v>
+      </c>
+      <c r="D13" t="s">
+        <v>120</v>
+      </c>
+    </row>
+    <row r="14" spans="1:4" x14ac:dyDescent="0.55000000000000004">
+      <c r="A14" t="s">
+        <v>27</v>
+      </c>
+      <c r="B14" t="s">
+        <v>30</v>
+      </c>
+      <c r="C14" s="2" t="s">
+        <v>31</v>
+      </c>
+      <c r="D14" t="s">
+        <v>120</v>
+      </c>
+    </row>
+    <row r="15" spans="1:4" x14ac:dyDescent="0.55000000000000004">
+      <c r="A15" t="s">
+        <v>27</v>
+      </c>
+      <c r="B15" t="s">
+        <v>121</v>
+      </c>
+      <c r="C15" s="7" t="s">
+        <v>32</v>
+      </c>
+      <c r="D15" t="s">
+        <v>120</v>
+      </c>
+    </row>
+    <row r="16" spans="1:4" x14ac:dyDescent="0.55000000000000004">
+      <c r="A16" t="s">
+        <v>27</v>
+      </c>
+      <c r="B16" t="s">
+        <v>33</v>
+      </c>
+      <c r="C16" s="2" t="s">
+        <v>34</v>
+      </c>
+      <c r="D16" t="s">
+        <v>120</v>
+      </c>
+    </row>
+    <row r="17" spans="1:4" x14ac:dyDescent="0.55000000000000004">
+      <c r="A17" t="s">
+        <v>27</v>
+      </c>
+      <c r="B17" t="s">
+        <v>35</v>
+      </c>
+      <c r="C17" s="2" t="s">
+        <v>36</v>
+      </c>
+      <c r="D17" t="s">
+        <v>120</v>
+      </c>
+    </row>
+    <row r="18" spans="1:4" x14ac:dyDescent="0.55000000000000004">
+      <c r="A18" t="s">
+        <v>27</v>
+      </c>
+      <c r="B18" t="s">
+        <v>37</v>
+      </c>
+      <c r="C18" s="2" t="s">
+        <v>38</v>
+      </c>
+      <c r="D18" t="s">
+        <v>120</v>
+      </c>
+    </row>
+    <row r="19" spans="1:4" x14ac:dyDescent="0.55000000000000004">
+      <c r="A19" t="s">
+        <v>27</v>
+      </c>
+      <c r="B19" t="s">
+        <v>39</v>
+      </c>
+      <c r="C19" s="2" t="s">
+        <v>40</v>
+      </c>
+      <c r="D19" t="s">
+        <v>120</v>
+      </c>
+    </row>
+    <row r="20" spans="1:4" x14ac:dyDescent="0.55000000000000004">
+      <c r="A20" t="s">
+        <v>27</v>
+      </c>
+      <c r="B20" t="s">
+        <v>41</v>
+      </c>
+      <c r="C20" s="2" t="s">
+        <v>42</v>
+      </c>
+      <c r="D20" t="s">
+        <v>120</v>
+      </c>
+    </row>
+    <row r="21" spans="1:4" x14ac:dyDescent="0.55000000000000004">
+      <c r="A21" t="s">
+        <v>27</v>
+      </c>
+      <c r="B21" t="s">
+        <v>43</v>
+      </c>
+      <c r="C21" s="2" t="s">
+        <v>44</v>
+      </c>
+      <c r="D21" t="s">
+        <v>120</v>
+      </c>
+    </row>
+    <row r="22" spans="1:4" x14ac:dyDescent="0.55000000000000004">
+      <c r="A22" t="s">
+        <v>27</v>
+      </c>
+      <c r="B22" t="s">
+        <v>45</v>
+      </c>
+      <c r="C22" s="2" t="s">
+        <v>46</v>
+      </c>
+      <c r="D22" t="s">
+        <v>120</v>
+      </c>
+    </row>
+    <row r="23" spans="1:4" x14ac:dyDescent="0.55000000000000004">
+      <c r="A23" t="s">
+        <v>27</v>
+      </c>
+      <c r="B23" t="s">
+        <v>47</v>
+      </c>
+      <c r="C23" s="2" t="s">
+        <v>48</v>
+      </c>
+      <c r="D23" t="s">
+        <v>120</v>
+      </c>
+    </row>
+    <row r="24" spans="1:4" x14ac:dyDescent="0.55000000000000004">
+      <c r="A24" t="s">
+        <v>27</v>
+      </c>
+      <c r="B24" t="s">
+        <v>49</v>
+      </c>
+      <c r="C24" s="2" t="s">
+        <v>50</v>
+      </c>
+      <c r="D24" t="s">
+        <v>120</v>
+      </c>
+    </row>
+    <row r="25" spans="1:4" x14ac:dyDescent="0.55000000000000004">
+      <c r="A25" t="s">
+        <v>27</v>
+      </c>
+      <c r="B25" t="s">
+        <v>51</v>
+      </c>
+      <c r="C25" s="2" t="s">
+        <v>52</v>
+      </c>
+      <c r="D25" t="s">
+        <v>120</v>
+      </c>
+    </row>
+    <row r="26" spans="1:4" x14ac:dyDescent="0.55000000000000004">
+      <c r="A26" t="s">
+        <v>27</v>
+      </c>
+      <c r="B26" t="s">
+        <v>53</v>
+      </c>
+      <c r="C26" s="2" t="s">
+        <v>54</v>
+      </c>
+      <c r="D26" t="s">
+        <v>120</v>
+      </c>
+    </row>
+    <row r="27" spans="1:4" x14ac:dyDescent="0.55000000000000004">
+      <c r="A27" t="s">
+        <v>27</v>
+      </c>
+      <c r="B27" t="s">
+        <v>55</v>
+      </c>
+      <c r="C27" s="2" t="s">
+        <v>56</v>
+      </c>
+      <c r="D27" t="s">
+        <v>120</v>
+      </c>
+    </row>
+    <row r="28" spans="1:4" x14ac:dyDescent="0.55000000000000004">
+      <c r="A28" t="s">
+        <v>27</v>
+      </c>
+      <c r="B28" t="s">
+        <v>57</v>
+      </c>
+      <c r="C28" s="2" t="s">
+        <v>58</v>
+      </c>
+      <c r="D28" t="s">
+        <v>120</v>
+      </c>
+    </row>
+    <row r="29" spans="1:4" x14ac:dyDescent="0.55000000000000004">
+      <c r="A29" t="s">
+        <v>27</v>
+      </c>
+      <c r="B29" t="s">
+        <v>59</v>
+      </c>
+      <c r="C29" s="2" t="s">
+        <v>60</v>
+      </c>
+      <c r="D29" t="s">
+        <v>120</v>
+      </c>
+    </row>
+    <row r="30" spans="1:4" x14ac:dyDescent="0.55000000000000004">
+      <c r="A30" t="s">
+        <v>27</v>
+      </c>
+      <c r="B30" t="s">
+        <v>61</v>
+      </c>
+      <c r="C30" s="2" t="s">
+        <v>62</v>
+      </c>
+      <c r="D30" t="s">
+        <v>120</v>
+      </c>
+    </row>
+    <row r="31" spans="1:4" x14ac:dyDescent="0.55000000000000004">
+      <c r="A31" t="s">
+        <v>27</v>
+      </c>
+      <c r="B31" t="s">
+        <v>63</v>
+      </c>
+      <c r="C31" s="2" t="s">
+        <v>64</v>
+      </c>
+      <c r="D31" t="s">
+        <v>120</v>
+      </c>
+    </row>
+    <row r="32" spans="1:4" x14ac:dyDescent="0.55000000000000004">
+      <c r="A32" t="s">
+        <v>27</v>
+      </c>
+      <c r="B32" t="s">
+        <v>65</v>
+      </c>
+      <c r="C32" s="3" t="s">
+        <v>66</v>
+      </c>
+      <c r="D32" t="s">
+        <v>120</v>
+      </c>
+    </row>
+    <row r="33" spans="1:4" x14ac:dyDescent="0.55000000000000004">
+      <c r="A33" t="s">
+        <v>27</v>
+      </c>
+      <c r="B33" t="s">
+        <v>67</v>
+      </c>
+      <c r="C33" s="2" t="s">
+        <v>68</v>
+      </c>
+      <c r="D33" t="s">
+        <v>120</v>
+      </c>
+    </row>
+    <row r="34" spans="1:4" x14ac:dyDescent="0.55000000000000004">
+      <c r="A34" t="s">
+        <v>27</v>
+      </c>
+      <c r="B34" t="s">
+        <v>69</v>
+      </c>
+      <c r="C34" s="2" t="s">
+        <v>70</v>
+      </c>
+      <c r="D34" t="s">
+        <v>120</v>
+      </c>
+    </row>
+    <row r="35" spans="1:4" x14ac:dyDescent="0.55000000000000004">
+      <c r="A35" t="s">
+        <v>27</v>
+      </c>
+      <c r="B35" t="s">
+        <v>71</v>
+      </c>
+      <c r="C35" s="2" t="s">
+        <v>72</v>
+      </c>
+      <c r="D35" t="s">
+        <v>120</v>
+      </c>
+    </row>
+    <row r="36" spans="1:4" x14ac:dyDescent="0.55000000000000004">
+      <c r="A36" t="s">
+        <v>27</v>
+      </c>
+      <c r="B36" t="s">
+        <v>73</v>
+      </c>
+      <c r="C36" s="2" t="s">
+        <v>74</v>
+      </c>
+      <c r="D36" t="s">
+        <v>120</v>
+      </c>
+    </row>
+    <row r="37" spans="1:4" x14ac:dyDescent="0.55000000000000004">
+      <c r="A37" t="s">
+        <v>27</v>
+      </c>
+      <c r="B37" t="s">
+        <v>75</v>
+      </c>
+      <c r="C37" s="2" t="s">
+        <v>76</v>
+      </c>
+      <c r="D37" t="s">
+        <v>120</v>
+      </c>
+    </row>
+    <row r="38" spans="1:4" x14ac:dyDescent="0.55000000000000004">
+      <c r="A38" t="s">
+        <v>27</v>
+      </c>
+      <c r="B38" t="s">
+        <v>77</v>
+      </c>
+      <c r="C38" s="2" t="s">
+        <v>78</v>
+      </c>
+      <c r="D38" t="s">
+        <v>120</v>
+      </c>
+    </row>
+    <row r="39" spans="1:4" x14ac:dyDescent="0.55000000000000004">
+      <c r="A39" t="s">
+        <v>27</v>
+      </c>
+      <c r="B39" t="s">
+        <v>79</v>
+      </c>
+      <c r="C39" s="2" t="s">
+        <v>80</v>
+      </c>
+      <c r="D39" t="s">
+        <v>120</v>
+      </c>
+    </row>
+    <row r="40" spans="1:4" x14ac:dyDescent="0.55000000000000004">
+      <c r="A40" t="s">
+        <v>27</v>
+      </c>
+      <c r="B40" t="s">
+        <v>81</v>
+      </c>
+      <c r="C40" s="2" t="s">
+        <v>82</v>
+      </c>
+      <c r="D40" t="s">
+        <v>120</v>
+      </c>
+    </row>
+    <row r="41" spans="1:4" x14ac:dyDescent="0.55000000000000004">
+      <c r="A41" t="s">
+        <v>27</v>
+      </c>
+      <c r="B41" t="s">
+        <v>83</v>
+      </c>
+      <c r="C41" s="2" t="s">
+        <v>84</v>
+      </c>
+      <c r="D41" t="s">
+        <v>120</v>
+      </c>
+    </row>
+    <row r="42" spans="1:4" x14ac:dyDescent="0.55000000000000004">
+      <c r="A42" t="s">
+        <v>27</v>
+      </c>
+      <c r="B42" t="s">
+        <v>85</v>
+      </c>
+      <c r="C42" s="2" t="s">
+        <v>86</v>
+      </c>
+      <c r="D42" t="s">
+        <v>120</v>
+      </c>
+    </row>
+    <row r="43" spans="1:4" x14ac:dyDescent="0.55000000000000004">
+      <c r="A43" t="s">
+        <v>27</v>
+      </c>
+      <c r="B43" t="s">
+        <v>122</v>
+      </c>
+      <c r="C43" s="3" t="s">
+        <v>87</v>
+      </c>
+      <c r="D43" t="s">
+        <v>120</v>
+      </c>
+    </row>
+    <row r="44" spans="1:4" x14ac:dyDescent="0.55000000000000004">
+      <c r="A44" t="s">
+        <v>27</v>
+      </c>
+      <c r="B44" s="4" t="s">
+        <v>88</v>
+      </c>
+      <c r="C44" s="6" t="s">
+        <v>89</v>
+      </c>
+      <c r="D44" t="s">
+        <v>120</v>
+      </c>
+    </row>
+    <row r="45" spans="1:4" x14ac:dyDescent="0.55000000000000004">
+      <c r="A45" s="4" t="s">
+        <v>8</v>
+      </c>
+      <c r="B45" t="s">
+        <v>15</v>
+      </c>
+      <c r="C45" t="s">
+        <v>21</v>
+      </c>
+      <c r="D45" t="s">
+        <v>120</v>
+      </c>
+    </row>
+    <row r="46" spans="1:4" x14ac:dyDescent="0.55000000000000004">
+      <c r="A46" s="4" t="s">
+        <v>8</v>
+      </c>
+      <c r="B46" t="s">
+        <v>16</v>
+      </c>
+      <c r="C46" t="s">
+        <v>22</v>
+      </c>
+      <c r="D46" t="s">
+        <v>120</v>
+      </c>
+    </row>
+    <row r="47" spans="1:4" x14ac:dyDescent="0.55000000000000004">
+      <c r="A47" s="4" t="s">
+        <v>8</v>
+      </c>
+      <c r="B47" t="s">
+        <v>17</v>
+      </c>
+      <c r="C47" t="s">
+        <v>23</v>
+      </c>
+      <c r="D47" t="s">
+        <v>120</v>
+      </c>
+    </row>
+    <row r="48" spans="1:4" x14ac:dyDescent="0.55000000000000004">
+      <c r="A48" s="4" t="s">
+        <v>8</v>
+      </c>
+      <c r="B48" t="s">
+        <v>18</v>
+      </c>
+      <c r="C48" s="2" t="s">
+        <v>24</v>
+      </c>
+      <c r="D48" t="s">
+        <v>120</v>
+      </c>
+    </row>
+    <row r="49" spans="1:4" x14ac:dyDescent="0.55000000000000004">
+      <c r="A49" s="4" t="s">
+        <v>8</v>
+      </c>
+      <c r="B49" s="4" t="s">
+        <v>19</v>
+      </c>
+      <c r="C49" s="5" t="s">
+        <v>25</v>
+      </c>
+      <c r="D49" t="s">
+        <v>120</v>
+      </c>
+    </row>
+    <row r="50" spans="1:4" x14ac:dyDescent="0.55000000000000004">
+      <c r="A50" s="4" t="s">
+        <v>8</v>
+      </c>
+      <c r="B50" s="5" t="s">
+        <v>91</v>
+      </c>
+      <c r="C50" s="2" t="s">
+        <v>90</v>
+      </c>
+      <c r="D50" t="s">
+        <v>120</v>
+      </c>
+    </row>
+    <row r="51" spans="1:4" x14ac:dyDescent="0.55000000000000004">
+      <c r="A51" s="4" t="s">
+        <v>8</v>
+      </c>
+      <c r="B51" s="5" t="s">
+        <v>92</v>
+      </c>
+      <c r="C51" s="2" t="s">
+        <v>29</v>
+      </c>
+      <c r="D51" t="s">
+        <v>120</v>
+      </c>
+    </row>
+    <row r="52" spans="1:4" x14ac:dyDescent="0.55000000000000004">
+      <c r="A52" s="4" t="s">
+        <v>8</v>
+      </c>
+      <c r="B52" s="5" t="s">
+        <v>94</v>
+      </c>
+      <c r="C52" s="2" t="s">
+        <v>93</v>
+      </c>
+      <c r="D52" t="s">
+        <v>120</v>
+      </c>
+    </row>
+    <row r="53" spans="1:4" x14ac:dyDescent="0.55000000000000004">
+      <c r="A53" s="4" t="s">
+        <v>8</v>
+      </c>
+      <c r="B53" s="5" t="s">
+        <v>96</v>
+      </c>
+      <c r="C53" s="2" t="s">
+        <v>95</v>
+      </c>
+      <c r="D53" t="s">
+        <v>120</v>
+      </c>
+    </row>
+    <row r="54" spans="1:4" x14ac:dyDescent="0.55000000000000004">
+      <c r="A54" s="4" t="s">
+        <v>8</v>
+      </c>
+      <c r="B54" s="5" t="s">
+        <v>98</v>
+      </c>
+      <c r="C54" s="2" t="s">
+        <v>97</v>
+      </c>
+      <c r="D54" t="s">
+        <v>120</v>
+      </c>
+    </row>
+    <row r="55" spans="1:4" x14ac:dyDescent="0.55000000000000004">
+      <c r="A55" s="4" t="s">
+        <v>8</v>
+      </c>
+      <c r="B55" t="s">
+        <v>99</v>
+      </c>
+      <c r="C55" s="4" t="s">
+        <v>26</v>
+      </c>
+      <c r="D55" t="s">
+        <v>120</v>
+      </c>
+    </row>
+    <row r="56" spans="1:4" x14ac:dyDescent="0.55000000000000004">
+      <c r="A56" s="4" t="s">
+        <v>8</v>
+      </c>
+      <c r="B56" s="4" t="s">
+        <v>100</v>
+      </c>
+      <c r="C56" s="5" t="s">
+        <v>54</v>
+      </c>
+      <c r="D56" t="s">
+        <v>120</v>
+      </c>
+    </row>
+    <row r="57" spans="1:4" x14ac:dyDescent="0.55000000000000004">
+      <c r="A57" s="4" t="s">
+        <v>8</v>
+      </c>
+      <c r="B57" t="s">
+        <v>55</v>
+      </c>
+      <c r="C57" s="2" t="s">
+        <v>56</v>
+      </c>
+      <c r="D57" t="s">
+        <v>120</v>
+      </c>
+    </row>
+    <row r="58" spans="1:4" x14ac:dyDescent="0.55000000000000004">
+      <c r="A58" s="4" t="s">
+        <v>8</v>
+      </c>
+      <c r="B58" t="s">
+        <v>57</v>
+      </c>
+      <c r="C58" s="2" t="s">
+        <v>58</v>
+      </c>
+      <c r="D58" t="s">
+        <v>120</v>
+      </c>
+    </row>
+    <row r="59" spans="1:4" x14ac:dyDescent="0.55000000000000004">
+      <c r="A59" s="4" t="s">
+        <v>8</v>
+      </c>
+      <c r="B59" t="s">
+        <v>59</v>
+      </c>
+      <c r="C59" s="2" t="s">
+        <v>60</v>
+      </c>
+      <c r="D59" t="s">
+        <v>120</v>
+      </c>
+    </row>
+    <row r="60" spans="1:4" x14ac:dyDescent="0.55000000000000004">
+      <c r="A60" s="4" t="s">
+        <v>8</v>
+      </c>
+      <c r="B60" t="s">
+        <v>61</v>
+      </c>
+      <c r="C60" s="2" t="s">
+        <v>62</v>
+      </c>
+      <c r="D60" t="s">
+        <v>120</v>
+      </c>
+    </row>
+    <row r="61" spans="1:4" x14ac:dyDescent="0.55000000000000004">
+      <c r="A61" s="4" t="s">
+        <v>8</v>
+      </c>
+      <c r="B61" s="4" t="s">
+        <v>63</v>
+      </c>
+      <c r="C61" s="5" t="s">
+        <v>64</v>
+      </c>
+      <c r="D61" t="s">
+        <v>120</v>
+      </c>
+    </row>
+    <row r="62" spans="1:4" x14ac:dyDescent="0.55000000000000004">
+      <c r="A62" s="4" t="s">
+        <v>8</v>
+      </c>
+      <c r="B62" t="s">
+        <v>37</v>
+      </c>
+      <c r="C62" s="2" t="s">
+        <v>38</v>
+      </c>
+      <c r="D62" t="s">
+        <v>120</v>
+      </c>
+    </row>
+    <row r="63" spans="1:4" x14ac:dyDescent="0.55000000000000004">
+      <c r="A63" s="4" t="s">
+        <v>8</v>
+      </c>
+      <c r="B63" t="s">
+        <v>39</v>
+      </c>
+      <c r="C63" s="2" t="s">
+        <v>40</v>
+      </c>
+      <c r="D63" t="s">
+        <v>120</v>
+      </c>
+    </row>
+    <row r="64" spans="1:4" x14ac:dyDescent="0.55000000000000004">
+      <c r="A64" s="4" t="s">
+        <v>8</v>
+      </c>
+      <c r="B64" t="s">
+        <v>41</v>
+      </c>
+      <c r="C64" s="2" t="s">
+        <v>42</v>
+      </c>
+      <c r="D64" t="s">
+        <v>120</v>
+      </c>
+    </row>
+    <row r="65" spans="1:4" x14ac:dyDescent="0.55000000000000004">
+      <c r="A65" s="4" t="s">
+        <v>8</v>
+      </c>
+      <c r="B65" t="s">
+        <v>43</v>
+      </c>
+      <c r="C65" s="2" t="s">
+        <v>44</v>
+      </c>
+      <c r="D65" t="s">
+        <v>120</v>
+      </c>
+    </row>
+    <row r="66" spans="1:4" x14ac:dyDescent="0.55000000000000004">
+      <c r="A66" s="4" t="s">
+        <v>8</v>
+      </c>
+      <c r="B66" t="s">
+        <v>45</v>
+      </c>
+      <c r="C66" s="2" t="s">
+        <v>46</v>
+      </c>
+      <c r="D66" t="s">
+        <v>120</v>
+      </c>
+    </row>
+    <row r="67" spans="1:4" x14ac:dyDescent="0.55000000000000004">
+      <c r="A67" s="4" t="s">
+        <v>8</v>
+      </c>
+      <c r="B67" t="s">
+        <v>47</v>
+      </c>
+      <c r="C67" s="2" t="s">
+        <v>48</v>
+      </c>
+      <c r="D67" t="s">
+        <v>120</v>
+      </c>
+    </row>
+    <row r="68" spans="1:4" x14ac:dyDescent="0.55000000000000004">
+      <c r="A68" s="4" t="s">
+        <v>8</v>
+      </c>
+      <c r="B68" t="s">
+        <v>49</v>
+      </c>
+      <c r="C68" s="2" t="s">
+        <v>50</v>
+      </c>
+      <c r="D68" t="s">
+        <v>120</v>
+      </c>
+    </row>
+    <row r="69" spans="1:4" x14ac:dyDescent="0.55000000000000004">
+      <c r="A69" s="4" t="s">
+        <v>8</v>
+      </c>
+      <c r="B69" s="4" t="s">
+        <v>51</v>
+      </c>
+      <c r="C69" s="5" t="s">
+        <v>52</v>
+      </c>
+      <c r="D69" t="s">
+        <v>120</v>
+      </c>
+    </row>
+    <row r="70" spans="1:4" x14ac:dyDescent="0.55000000000000004">
+      <c r="A70" s="4" t="s">
+        <v>8</v>
+      </c>
+      <c r="B70" t="s">
+        <v>102</v>
+      </c>
+      <c r="C70" s="4" t="s">
+        <v>101</v>
+      </c>
+      <c r="D70" t="s">
+        <v>120</v>
+      </c>
+    </row>
+    <row r="71" spans="1:4" x14ac:dyDescent="0.55000000000000004">
+      <c r="A71" s="4" t="s">
+        <v>8</v>
+      </c>
+      <c r="B71" s="4" t="s">
+        <v>104</v>
+      </c>
+      <c r="C71" s="5" t="s">
+        <v>103</v>
+      </c>
+      <c r="D71" t="s">
+        <v>120</v>
+      </c>
+    </row>
+    <row r="72" spans="1:4" x14ac:dyDescent="0.55000000000000004">
+      <c r="A72" s="4" t="s">
+        <v>8</v>
+      </c>
+      <c r="B72" s="4" t="s">
+        <v>106</v>
+      </c>
+      <c r="C72" s="5" t="s">
+        <v>105</v>
+      </c>
+      <c r="D72" t="s">
+        <v>120</v>
+      </c>
+    </row>
+    <row r="73" spans="1:4" x14ac:dyDescent="0.55000000000000004">
+      <c r="A73" s="4" t="s">
+        <v>8</v>
+      </c>
+      <c r="B73" s="5" t="s">
+        <v>107</v>
+      </c>
+      <c r="C73" s="5" t="s">
+        <v>108</v>
+      </c>
+      <c r="D73" t="s">
+        <v>120</v>
+      </c>
+    </row>
+    <row r="74" spans="1:4" x14ac:dyDescent="0.55000000000000004">
+      <c r="A74" s="4" t="s">
+        <v>8</v>
+      </c>
+      <c r="B74" s="4" t="s">
+        <v>110</v>
+      </c>
+      <c r="C74" s="5" t="s">
+        <v>109</v>
+      </c>
+      <c r="D74" t="s">
+        <v>120</v>
+      </c>
+    </row>
+    <row r="75" spans="1:4" x14ac:dyDescent="0.55000000000000004">
+      <c r="A75" s="4" t="s">
+        <v>8</v>
+      </c>
+      <c r="B75" s="4" t="s">
+        <v>112</v>
+      </c>
+      <c r="C75" s="5" t="s">
+        <v>111</v>
+      </c>
+      <c r="D75" t="s">
+        <v>120</v>
+      </c>
+    </row>
+    <row r="76" spans="1:4" x14ac:dyDescent="0.55000000000000004">
+      <c r="A76" s="4" t="s">
+        <v>8</v>
+      </c>
+      <c r="B76" s="4" t="s">
+        <v>113</v>
+      </c>
+      <c r="C76" s="5" t="s">
+        <v>114</v>
+      </c>
+      <c r="D76" t="s">
+        <v>120</v>
+      </c>
+    </row>
+    <row r="77" spans="1:4" x14ac:dyDescent="0.55000000000000004">
+      <c r="A77" s="4" t="s">
+        <v>8</v>
+      </c>
+      <c r="B77" s="4" t="s">
+        <v>116</v>
+      </c>
+      <c r="C77" s="5" t="s">
+        <v>115</v>
+      </c>
+      <c r="D77" t="s">
+        <v>120</v>
+      </c>
+    </row>
+    <row r="78" spans="1:4" x14ac:dyDescent="0.55000000000000004">
+      <c r="A78" s="4" t="s">
+        <v>8</v>
+      </c>
+      <c r="B78" s="4" t="s">
+        <v>118</v>
+      </c>
+      <c r="C78" s="5" t="s">
+        <v>117</v>
+      </c>
+      <c r="D78" t="s">
+        <v>120</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
+  <tableParts count="1">
+    <tablePart r:id="rId2"/>
+  </tableParts>
+</worksheet>
+</file>
+
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
-<ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Document" ma:contentTypeID="0x010100078FB844456CC1439CE7A159479264B8" ma:contentTypeVersion="5" ma:contentTypeDescription="Create a new document." ma:contentTypeScope="" ma:versionID="996a4699cbb302f4d95a15d67d32f7e1">
-  <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns2="df49477f-2fdb-440d-ba1e-675744a510a7" xmlns:ns3="272bea84-3b1f-4555-a3af-524feb91c688" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="ebe6ffb6dba8b9d24d4c1cd32a9bdc8d" ns2:_="" ns3:_="">
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
+</file>
+
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
+<ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Document" ma:contentTypeID="0x010100078FB844456CC1439CE7A159479264B8" ma:contentTypeVersion="11" ma:contentTypeDescription="Create a new document." ma:contentTypeScope="" ma:versionID="1c8f7bf46c6ea8358ae2988c9d2e2891">
+  <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns2="df49477f-2fdb-440d-ba1e-675744a510a7" xmlns:ns3="272bea84-3b1f-4555-a3af-524feb91c688" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="d81c36c5695409b08a7e45d9dfe44ecd" ns2:_="" ns3:_="">
     <xsd:import namespace="df49477f-2fdb-440d-ba1e-675744a510a7"/>
     <xsd:import namespace="272bea84-3b1f-4555-a3af-524feb91c688"/>
     <xsd:element name="properties">
@@ -545,6 +2130,11 @@
                 <xsd:element ref="ns3:SharedWithUsers" minOccurs="0"/>
                 <xsd:element ref="ns3:SharedWithDetails" minOccurs="0"/>
                 <xsd:element ref="ns2:MediaServiceObjectDetectorVersions" minOccurs="0"/>
+                <xsd:element ref="ns2:lcf76f155ced4ddcb4097134ff3c332f" minOccurs="0"/>
+                <xsd:element ref="ns3:TaxCatchAll" minOccurs="0"/>
+                <xsd:element ref="ns2:MediaServiceOCR" minOccurs="0"/>
+                <xsd:element ref="ns2:MediaServiceGenerationTime" minOccurs="0"/>
+                <xsd:element ref="ns2:MediaServiceEventHashCode" minOccurs="0"/>
               </xsd:all>
             </xsd:complexType>
           </xsd:element>
@@ -566,6 +2156,30 @@
       </xsd:simpleType>
     </xsd:element>
     <xsd:element name="MediaServiceObjectDetectorVersions" ma:index="12" nillable="true" ma:displayName="MediaServiceObjectDetectorVersions" ma:hidden="true" ma:indexed="true" ma:internalName="MediaServiceObjectDetectorVersions" ma:readOnly="true">
+      <xsd:simpleType>
+        <xsd:restriction base="dms:Text"/>
+      </xsd:simpleType>
+    </xsd:element>
+    <xsd:element name="lcf76f155ced4ddcb4097134ff3c332f" ma:index="14" nillable="true" ma:taxonomy="true" ma:internalName="lcf76f155ced4ddcb4097134ff3c332f" ma:taxonomyFieldName="MediaServiceImageTags" ma:displayName="Image Tags" ma:readOnly="false" ma:fieldId="{5cf76f15-5ced-4ddc-b409-7134ff3c332f}" ma:taxonomyMulti="true" ma:sspId="5acc4dc2-1d7d-4ba2-9bc5-748c4ad50a69" ma:termSetId="09814cd3-568e-fe90-9814-8d621ff8fb84" ma:anchorId="fba54fb3-c3e1-fe81-a776-ca4b69148c4d" ma:open="true" ma:isKeyword="false">
+      <xsd:complexType>
+        <xsd:sequence>
+          <xsd:element ref="pc:Terms" minOccurs="0" maxOccurs="1"/>
+        </xsd:sequence>
+      </xsd:complexType>
+    </xsd:element>
+    <xsd:element name="MediaServiceOCR" ma:index="16" nillable="true" ma:displayName="Extracted Text" ma:internalName="MediaServiceOCR" ma:readOnly="true">
+      <xsd:simpleType>
+        <xsd:restriction base="dms:Note">
+          <xsd:maxLength value="255"/>
+        </xsd:restriction>
+      </xsd:simpleType>
+    </xsd:element>
+    <xsd:element name="MediaServiceGenerationTime" ma:index="17" nillable="true" ma:displayName="MediaServiceGenerationTime" ma:hidden="true" ma:internalName="MediaServiceGenerationTime" ma:readOnly="true">
+      <xsd:simpleType>
+        <xsd:restriction base="dms:Text"/>
+      </xsd:simpleType>
+    </xsd:element>
+    <xsd:element name="MediaServiceEventHashCode" ma:index="18" nillable="true" ma:displayName="MediaServiceEventHashCode" ma:hidden="true" ma:internalName="MediaServiceEventHashCode" ma:readOnly="true">
       <xsd:simpleType>
         <xsd:restriction base="dms:Text"/>
       </xsd:simpleType>
@@ -599,6 +2213,17 @@
           <xsd:maxLength value="255"/>
         </xsd:restriction>
       </xsd:simpleType>
+    </xsd:element>
+    <xsd:element name="TaxCatchAll" ma:index="15" nillable="true" ma:displayName="Taxonomy Catch All Column" ma:hidden="true" ma:list="{60e743a2-b3c6-4343-b1f6-389c769eaba6}" ma:internalName="TaxCatchAll" ma:showField="CatchAllData" ma:web="272bea84-3b1f-4555-a3af-524feb91c688">
+      <xsd:complexType>
+        <xsd:complexContent>
+          <xsd:extension base="dms:MultiChoiceLookup">
+            <xsd:sequence>
+              <xsd:element name="Value" type="dms:Lookup" maxOccurs="unbounded" minOccurs="0" nillable="true"/>
+            </xsd:sequence>
+          </xsd:extension>
+        </xsd:complexContent>
+      </xsd:complexType>
     </xsd:element>
   </xsd:schema>
   <xsd:schema xmlns="http://schemas.openxmlformats.org/package/2006/metadata/core-properties" xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:dc="http://purl.org/dc/elements/1.1/" xmlns:dcterms="http://purl.org/dc/terms/" xmlns:odoc="http://schemas.microsoft.com/internal/obd" targetNamespace="http://schemas.openxmlformats.org/package/2006/metadata/core-properties" elementFormDefault="qualified" attributeFormDefault="unqualified" blockDefault="#all">
@@ -700,23 +2325,27 @@
 </ct:contentTypeSchema>
 </file>
 
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement/>
+  <documentManagement>
+    <TaxCatchAll xmlns="272bea84-3b1f-4555-a3af-524feb91c688" xsi:nil="true"/>
+    <lcf76f155ced4ddcb4097134ff3c332f xmlns="df49477f-2fdb-440d-ba1e-675744a510a7">
+      <Terms xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    </lcf76f155ced4ddcb4097134ff3c332f>
+  </documentManagement>
 </p:properties>
 </file>
 
-<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
+<file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{C4C492B7-1129-41A1-824F-AF2B4F0C3BD3}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
 
-<file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{40D87B69-39D5-493B-A16C-F1F1A2E9E303}">
+<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{C81BD1EA-27C3-482A-B745-6355F997FCA2}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes"/>
@@ -734,19 +2363,13 @@
 </ds:datastoreItem>
 </file>
 
-<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{BF3E4F3B-1E48-447B-9CCB-C7ABB5D25424}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{C4C492B7-1129-41A1-824F-AF2B4F0C3BD3}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+    <ds:schemaRef ds:uri="272bea84-3b1f-4555-a3af-524feb91c688"/>
+    <ds:schemaRef ds:uri="df49477f-2fdb-440d-ba1e-675744a510a7"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
 </file>
</xml_diff>